<commit_message>
some fixes to Tableau
</commit_message>
<xml_diff>
--- a/GHATIM/DataSpreadsheets/EnergyPriceChecks.xlsx
+++ b/GHATIM/DataSpreadsheets/EnergyPriceChecks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\GHATIMGE\GHATIM\DataSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4166959-52D7-48A4-A63F-5891FFF6E05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2D0FD0-63DA-4B75-82DD-5D3EF34CF70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="45" windowWidth="28770" windowHeight="15600" xr2:uid="{06280540-0903-4C89-B0EA-0461296BF0DA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="15600" xr2:uid="{06280540-0903-4C89-B0EA-0461296BF0DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>Electricity Price</t>
   </si>
@@ -56,9 +56,6 @@
     <t xml:space="preserve">Source: </t>
   </si>
   <si>
-    <t>Model b$/PJ</t>
-  </si>
-  <si>
     <t>.216-&gt;.13</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>216-130</t>
   </si>
   <si>
-    <t>b$/PJ</t>
-  </si>
-  <si>
     <t>cpetr</t>
   </si>
   <si>
@@ -87,6 +81,15 @@
   </si>
   <si>
     <t>GJ/l</t>
+  </si>
+  <si>
+    <t>Model bGC/PJ</t>
+  </si>
+  <si>
+    <t>GC/GJ</t>
+  </si>
+  <si>
+    <t>exchange rate</t>
   </si>
 </sst>
 </file>
@@ -125,10 +128,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,13 +628,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6DE878A-AE64-4391-8D01-B83A7BB99CC7}">
-  <dimension ref="C3:P51"/>
+  <dimension ref="C2:R51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="11" ySplit="4" topLeftCell="L20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="4" topLeftCell="L25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="M51" sqref="M51:N51"/>
+      <selection pane="bottomRight" activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +642,16 @@
     <col min="14" max="14" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2">
+        <f>0.541/0.147</f>
+        <v>3.6802721088435377</v>
+      </c>
+    </row>
+    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -646,7 +659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
       <c r="L4" t="s">
         <v>1</v>
       </c>
@@ -654,13 +667,16 @@
         <v>2</v>
       </c>
       <c r="O4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="P4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
       <c r="K18">
         <v>2015</v>
       </c>
@@ -672,13 +688,21 @@
         <v>40.833333333333336</v>
       </c>
       <c r="O18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="Q18" s="2">
+        <f>216/3.7</f>
+        <v>58.378378378378379</v>
+      </c>
+      <c r="R18" s="3">
+        <f>130/3.7</f>
+        <v>35.135135135135137</v>
+      </c>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>3</v>
       </c>
@@ -686,21 +710,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
       <c r="L27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M27" t="s">
         <v>2</v>
       </c>
       <c r="O27" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="P27" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q27" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
       <c r="K28">
         <v>2015</v>
       </c>
@@ -717,24 +744,28 @@
       <c r="P28">
         <v>32</v>
       </c>
+      <c r="Q28">
+        <f>P28/3.7</f>
+        <v>8.6486486486486474</v>
+      </c>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D35" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="3:14" x14ac:dyDescent="0.25">
       <c r="M48" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="N48" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="11:16" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="11:17" x14ac:dyDescent="0.25">
       <c r="M49">
         <v>36</v>
       </c>
@@ -743,24 +774,27 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="50" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="11:17" x14ac:dyDescent="0.25">
       <c r="L50" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M50" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N50" t="s">
         <v>2</v>
       </c>
       <c r="O50" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="P50" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q50" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K51">
         <v>2015</v>
       </c>
@@ -768,12 +802,12 @@
         <v>297</v>
       </c>
       <c r="M51" s="1">
-        <f>0.147/0.541*L51</f>
-        <v>80.700554528650628</v>
+        <f>0.147/0.541*L51/100</f>
+        <v>0.80700554528650625</v>
       </c>
       <c r="N51" s="1">
-        <f>M51*N49</f>
-        <v>2.9052199630314224</v>
+        <f>M51/N49</f>
+        <v>22.416820702402955</v>
       </c>
       <c r="O51">
         <v>1.466</v>
@@ -781,6 +815,10 @@
       <c r="P51">
         <f>O51*1000</f>
         <v>1466</v>
+      </c>
+      <c r="Q51">
+        <f>P51/3.7</f>
+        <v>396.2162162162162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates made on emissions. CO2 scenario implemented
</commit_message>
<xml_diff>
--- a/GHATIM/DataSpreadsheets/EnergyPriceChecks.xlsx
+++ b/GHATIM/DataSpreadsheets/EnergyPriceChecks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\GHATIMGE\GHATIM\DataSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2D0FD0-63DA-4B75-82DD-5D3EF34CF70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FE1BC5-0A18-477C-A674-C6475B69004B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="15600" xr2:uid="{06280540-0903-4C89-B0EA-0461296BF0DA}"/>
+    <workbookView xWindow="2940" yWindow="-16815" windowWidth="28770" windowHeight="15600" xr2:uid="{06280540-0903-4C89-B0EA-0461296BF0DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Electricity Price</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>exchange rate</t>
+  </si>
+  <si>
+    <t>GC/$</t>
   </si>
 </sst>
 </file>
@@ -97,7 +100,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -131,7 +134,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -620,7 +623,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -634,7 +637,7 @@
       <pane xSplit="11" ySplit="4" topLeftCell="L25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N51" sqref="N51"/>
+      <selection pane="bottomRight" activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,8 +646,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2">
         <f>0.541/0.147</f>
@@ -745,8 +751,8 @@
         <v>32</v>
       </c>
       <c r="Q28">
-        <f>P28/3.7</f>
-        <v>8.6486486486486474</v>
+        <f>P28/J2</f>
+        <v>8.6950092421441774</v>
       </c>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.25">
@@ -802,8 +808,8 @@
         <v>297</v>
       </c>
       <c r="M51" s="1">
-        <f>0.147/0.541*L51/100</f>
-        <v>0.80700554528650625</v>
+        <f>L51/J2/100</f>
+        <v>0.80700554528650636</v>
       </c>
       <c r="N51" s="1">
         <f>M51/N49</f>
@@ -817,8 +823,8 @@
         <v>1466</v>
       </c>
       <c r="Q51">
-        <f>P51/3.7</f>
-        <v>396.2162162162162</v>
+        <f>P51/J2</f>
+        <v>398.34011090573011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>